<commit_message>
WRI Updates to HK model from 11/15
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
+++ b/InputData/add-outputs/VoaSL/Value of a Statistical Life.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\VoaSL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\World Resources Institute\TRAC City - HK 2050 is now\eps-1.4.3-hk-wipB\eps-1.4.3-hk-wipB\InputData\add-outputs\VoaSL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_AB7C9A337BB36FE76E84E66B932EE341CB00D162" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4FB19959-348F-407C-A9FD-793088147DC4}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="24915" windowHeight="11580"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="VoaSL" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="4" r:id="rId2"/>
+    <sheet name="VoaSL" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -28,55 +38,55 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>U.S. Environmental Protection Agency</t>
-  </si>
-  <si>
-    <t>http://yosemite.epa.gov/EE%5Cepa%5Ceed.nsf/webpages/MortalityRiskValuation.html#whatvalue</t>
-  </si>
-  <si>
-    <t>Frequently Asked Questions on Mortality Risk Valuation</t>
-  </si>
-  <si>
-    <t>We adjust 2006 dollars to 2012 dollars using the following conversion factor:</t>
-  </si>
-  <si>
-    <t>See "cpi.xlsx" in the InputData folder for source information.</t>
+    <t>Hua Wang and Jie He, World Bank Development Research Group</t>
+  </si>
+  <si>
+    <t>The Value of Statistical Life : A Contingent Investigation in China</t>
+  </si>
+  <si>
+    <t>https://openknowledge.worldbank.org/handle/10986/3905</t>
+  </si>
+  <si>
+    <t>Abstract</t>
   </si>
   <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>"What value of statistical life does EPA use?"</t>
+    <t>This variable is used to convert from dollars (in the SCoHIbP Social Cost of</t>
+  </si>
+  <si>
+    <t>Health Impacts by Pollutant variable) into human lives, so the VSL figure</t>
+  </si>
+  <si>
+    <t>here must reflect the one used to calculate the health impacts in that</t>
+  </si>
+  <si>
+    <t>variable for the result to be accurate.</t>
+  </si>
+  <si>
+    <t>China VoaSL data</t>
+  </si>
+  <si>
+    <t>yuan</t>
+  </si>
+  <si>
+    <t>dollars per yuan</t>
+  </si>
+  <si>
+    <t>USD</t>
   </si>
   <si>
     <t>Statistical Life</t>
   </si>
   <si>
-    <t>This variable is used to convert from dollars (in the SCoHIbP Social Cost of</t>
-  </si>
-  <si>
-    <t>Health Impacts by Pollutant variable) into human lives, so the VSL figure</t>
-  </si>
-  <si>
-    <t>here must reflect the one used to calculate the health impacts in that</t>
-  </si>
-  <si>
-    <t>variable for the result to be accurate.</t>
-  </si>
-  <si>
-    <t>Currency Year Adjustment</t>
-  </si>
-  <si>
-    <t>2012$/life</t>
-  </si>
-  <si>
-    <t>Value</t>
+    <t>Value (2012$)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,7 +133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -134,6 +144,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -228,6 +239,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -263,6 +291,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,10 +483,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -463,70 +510,106 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>2013</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{C8A0D264-030B-4C66-9744-137C1B55BFB9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>795000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.14573</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <f>A3*A5</f>
+        <v>115855.35</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.141</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -535,15 +618,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,20 +636,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="B1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
-        <f>7.4*10^6*About!A17</f>
-        <v>8443400</v>
+      <c r="B2" s="6">
+        <f>Data!A7</f>
+        <v>115855.35</v>
       </c>
     </row>
   </sheetData>
@@ -827,13 +907,31 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01D78074-3962-4EB3-B017-93329FD0570B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E7781F9-6353-4A61-823B-CE6E96243302}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F820317A-01E7-43D2-81DB-3C9D92798BA3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7ABCA70-D359-45C2-BB14-0B78385CACBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B564D760-F6F5-4CFD-8462-776C1D9E6B8E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C035858-B5F2-4371-B64A-296D500AB545}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="c9df191c-55f2-496b-9838-9a5abe4742ad"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7889d872-e2a2-4afb-87bc-97561eced75f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>